<commit_message>
Implement changes requested by Fikri
</commit_message>
<xml_diff>
--- a/src/pypelay/options.xlsx
+++ b/src/pypelay/options.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daveh\Github\J017-Sapura\working\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daveh\Github\J017-Sapura\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0417908B-300B-4CBC-A161-4742E1401D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81965D21-22B5-407B-98AC-124557D448CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{74D002A0-BFA5-4336-949D-C5BB6DB23233}"/>
+    <workbookView xWindow="3900" yWindow="1350" windowWidth="22305" windowHeight="14295" xr2:uid="{74D002A0-BFA5-4336-949D-C5BB6DB23233}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>Stinger tip definition</t>
   </si>
@@ -78,28 +78,13 @@
     <t>m</t>
   </si>
   <si>
-    <t>Top tension option</t>
-  </si>
-  <si>
     <t>Default is 10t for top tension &lt; 100t, otherwise 10%</t>
   </si>
   <si>
     <t>Comment</t>
   </si>
   <si>
-    <t>User input in t</t>
-  </si>
-  <si>
-    <t>No rounding</t>
-  </si>
-  <si>
-    <t>Round to nearest 5t</t>
-  </si>
-  <si>
     <t>For % top tension enter number between 0 and 1</t>
-  </si>
-  <si>
-    <t>Round up to nearest 5t</t>
   </si>
   <si>
     <t>% or t</t>
@@ -533,7 +518,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,7 +533,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>9</v>
@@ -560,7 +545,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -591,7 +576,7 @@
         <v>20</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -599,7 +584,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>12</v>
@@ -650,7 +635,7 @@
         <v>100</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -664,10 +649,10 @@
         <v>11</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -675,34 +660,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D9" s="3">
+        <v>5</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1A0B828D-8024-4F21-8477-FC2C253D24DB}">
           <x14:formula1>
             <xm:f>Sheet2!$C$5:$C$8</xm:f>
           </x14:formula1>
           <xm:sqref>D8</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4E904726-AA1E-4FFB-83F3-A4B751D48C12}">
-          <x14:formula1>
-            <xm:f>Sheet2!$C$10:$C$13</xm:f>
-          </x14:formula1>
-          <xm:sqref>D10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FC1D4E8B-08CE-41D1-AC10-312CE981A2C6}">
           <x14:formula1>
@@ -718,10 +697,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1153DDF-E404-48CA-A4BB-1994F69232A3}">
-  <dimension ref="B2:C13"/>
+  <dimension ref="B2:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,40 +728,17 @@
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add CWC for static results. Important bugfix to get_roller_heights
</commit_message>
<xml_diff>
--- a/src/pypelay/options.xlsx
+++ b/src/pypelay/options.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daveh\Github\J017-Sapura\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daveh\Github\J017-Sapura\pypelay\src\pypelay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81965D21-22B5-407B-98AC-124557D448CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF72C23-24DD-46ED-A4BE-63ECCDD7E823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="1350" windowWidth="22305" windowHeight="14295" xr2:uid="{74D002A0-BFA5-4336-949D-C5BB6DB23233}"/>
+    <workbookView xWindow="9705" yWindow="1875" windowWidth="16800" windowHeight="13170" xr2:uid="{74D002A0-BFA5-4336-949D-C5BB6DB23233}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -118,6 +118,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -161,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -180,6 +183,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -515,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02C2E2EF-C952-4851-98E7-DF37EE700BF8}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,6 +677,9 @@
       <c r="E9" s="4" t="s">
         <v>15</v>
       </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>